<commit_message>
added start end time
</commit_message>
<xml_diff>
--- a/data/data_sub.xlsx
+++ b/data/data_sub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\code_tesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF69999-B528-4C7B-9283-2A553D8DCEC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1315C69-8E6F-4853-9028-D3B82B1FF5EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1188" yWindow="-108" windowWidth="21960" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,11 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -745,6 +741,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1102,147 +1102,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35062D11-4130-4812-8D10-4AE0B319C1E7}">
   <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
     <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" customWidth="1"/>
     <col min="19" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" customWidth="1"/>
+    <col min="22" max="22" width="8.77734375" customWidth="1"/>
+    <col min="23" max="23" width="5.88671875" customWidth="1"/>
+    <col min="24" max="24" width="9.109375" customWidth="1"/>
     <col min="25" max="25" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.88671875" customWidth="1"/>
+    <col min="28" max="28" width="8.33203125" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" customWidth="1"/>
+    <col min="30" max="30" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="18" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="16" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16" t="s">
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="18" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="18" t="s">
+      <c r="N2" s="18"/>
+      <c r="O2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18" t="s">
+      <c r="P2" s="18"/>
+      <c r="Q2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="16" t="s">
+      <c r="R2" s="18"/>
+      <c r="S2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16" t="s">
+      <c r="T2" s="15"/>
+      <c r="U2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="16"/>
-      <c r="W2" s="17" t="s">
+      <c r="V2" s="15"/>
+      <c r="W2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16" t="s">
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16" t="s">
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="17" t="s">
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AD2" s="16"/>
+      <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -1355,19 +1355,19 @@
       <c r="F4" s="4">
         <v>100</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>200</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4">
-        <v>200</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>200</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3">
+        <v>200</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="4">
@@ -1447,19 +1447,19 @@
       <c r="F5" s="4">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>50</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3">
+        <v>50</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="3">
+        <v>50</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="4">
@@ -1539,19 +1539,19 @@
       <c r="F6" s="4">
         <v>50</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>100</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3">
+        <v>100</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3">
+        <v>100</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="4">
@@ -1631,19 +1631,19 @@
       <c r="F7" s="4">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>30</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="4">
@@ -1723,19 +1723,19 @@
       <c r="F8" s="4">
         <v>200</v>
       </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="4">
@@ -1815,19 +1815,19 @@
       <c r="F9" s="4">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="15">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="19">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="4">
@@ -1907,19 +1907,19 @@
       <c r="F10" s="4">
         <v>200</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L10" s="4">
@@ -1999,19 +1999,19 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>200</v>
-      </c>
-      <c r="I11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11">
-        <v>200</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>200</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
+        <v>200</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L11" s="4">
@@ -2091,19 +2091,19 @@
       <c r="F12" s="4">
         <v>50</v>
       </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
-        <v>50</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <v>50</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3">
+        <v>50</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3">
+        <v>50</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="4">
@@ -2183,19 +2183,19 @@
       <c r="F13" s="4">
         <v>3</v>
       </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13">
-        <v>30</v>
-      </c>
-      <c r="I13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="3">
+        <v>30</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="3">
+        <v>30</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L13" s="4">
@@ -2275,19 +2275,19 @@
       <c r="F14" s="4">
         <v>200</v>
       </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14">
-        <v>100</v>
-      </c>
-      <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14">
-        <v>100</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>100</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="3">
+        <v>100</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L14" s="4">
@@ -2367,19 +2367,19 @@
       <c r="F15" s="4">
         <v>100</v>
       </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15">
-        <v>10</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3">
+        <v>10</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>10</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="4">
@@ -2459,19 +2459,19 @@
       <c r="F16" s="4">
         <v>30</v>
       </c>
-      <c r="G16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L16" s="4">
@@ -2551,19 +2551,19 @@
       <c r="F17" s="4">
         <v>3</v>
       </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>100</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>100</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3">
+        <v>100</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="3">
+        <v>100</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L17" s="4">
@@ -2643,19 +2643,19 @@
       <c r="F18" s="4">
         <v>10</v>
       </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>10</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3">
+        <v>10</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <v>10</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L18" s="4">
@@ -2735,19 +2735,19 @@
       <c r="F19" s="4">
         <v>30</v>
       </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="3">
+        <v>30</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="3">
+        <v>30</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L19" s="4">
@@ -2827,19 +2827,19 @@
       <c r="F20" s="4">
         <v>100</v>
       </c>
-      <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20">
-        <v>50</v>
-      </c>
-      <c r="I20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20">
-        <v>50</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="3">
+        <v>50</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L20" s="4">
@@ -2919,19 +2919,19 @@
       <c r="F21" s="4">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>200</v>
-      </c>
-      <c r="I21" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21">
-        <v>200</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="G21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>200</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="3">
+        <v>200</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L21" s="4">
@@ -3011,19 +3011,19 @@
       <c r="F22" s="4">
         <v>100</v>
       </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22">
-        <v>3</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L22" s="4">
@@ -3103,19 +3103,19 @@
       <c r="F23" s="4">
         <v>10</v>
       </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23">
-        <v>10</v>
-      </c>
-      <c r="I23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23">
-        <v>10</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="3">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>10</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L23" s="4">
@@ -3195,19 +3195,19 @@
       <c r="F24" s="4">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24">
-        <v>30</v>
-      </c>
-      <c r="I24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24">
-        <v>30</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="G24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="3">
+        <v>30</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="3">
+        <v>30</v>
+      </c>
+      <c r="K24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L24" s="4">
@@ -3287,19 +3287,19 @@
       <c r="F25" s="4">
         <v>30</v>
       </c>
-      <c r="G25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25">
-        <v>200</v>
-      </c>
-      <c r="I25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J25">
-        <v>200</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="G25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3">
+        <v>200</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="3">
+        <v>200</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L25" s="4">
@@ -3379,19 +3379,19 @@
       <c r="F26" s="4">
         <v>200</v>
       </c>
-      <c r="G26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26">
-        <v>50</v>
-      </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <v>50</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="3">
+        <v>50</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="3">
+        <v>50</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L26" s="4">
@@ -3471,19 +3471,19 @@
       <c r="F27" s="4">
         <v>10</v>
       </c>
-      <c r="G27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27">
-        <v>100</v>
-      </c>
-      <c r="I27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27">
-        <v>100</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>100</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="3">
+        <v>100</v>
+      </c>
+      <c r="K27" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L27" s="4">
@@ -3563,19 +3563,19 @@
       <c r="F28" s="4">
         <v>200</v>
       </c>
-      <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28">
-        <v>10</v>
-      </c>
-      <c r="I28" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28">
-        <v>10</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="3">
+        <v>10</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="3">
+        <v>10</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L28" s="4">
@@ -3655,19 +3655,19 @@
       <c r="F29" s="4">
         <v>3</v>
       </c>
-      <c r="G29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29">
-        <v>30</v>
-      </c>
-      <c r="I29" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29">
-        <v>30</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="3">
+        <v>30</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3">
+        <v>30</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L29" s="4">
@@ -3747,19 +3747,19 @@
       <c r="F30" s="4">
         <v>50</v>
       </c>
-      <c r="G30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30">
-        <v>200</v>
-      </c>
-      <c r="I30" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30">
-        <v>200</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="3">
+        <v>200</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="3">
+        <v>200</v>
+      </c>
+      <c r="K30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L30" s="4">
@@ -3839,19 +3839,19 @@
       <c r="F31" s="4">
         <v>3</v>
       </c>
-      <c r="G31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31">
-        <v>50</v>
-      </c>
-      <c r="I31" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31">
-        <v>50</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="G31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="3">
+        <v>50</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" s="3">
+        <v>50</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L31" s="4">
@@ -3931,19 +3931,19 @@
       <c r="F32" s="4">
         <v>100</v>
       </c>
-      <c r="G32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32">
-        <v>100</v>
-      </c>
-      <c r="I32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32">
-        <v>100</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="G32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="3">
+        <v>100</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="3">
+        <v>100</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L32" s="4">
@@ -4023,19 +4023,19 @@
       <c r="F33" s="9">
         <v>30</v>
       </c>
-      <c r="G33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33">
-        <v>3</v>
-      </c>
-      <c r="I33" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33">
-        <v>3</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="G33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="8">
+        <v>3</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="8">
+        <v>3</v>
+      </c>
+      <c r="K33" s="8" t="s">
         <v>5</v>
       </c>
       <c r="L33" s="9">
@@ -4098,6 +4098,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="M1:R1"/>
     <mergeCell ref="S1:X1"/>
@@ -4114,10 +4118,6 @@
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4129,134 +4129,134 @@
   <dimension ref="A1:AR33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16" t="s">
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="16" t="s">
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16" t="s">
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="17" t="s">
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16" t="s">
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16" t="s">
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="17" t="s">
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+      <c r="AP2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AQ2" s="16"/>
-      <c r="AR2" s="16"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="15"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -8294,6 +8294,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AH1:AR1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AE2:AG2"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="L1:V1"/>
     <mergeCell ref="W1:AG1"/>
@@ -8305,11 +8310,6 @@
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AH1:AR1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AE2:AG2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8372,128 +8372,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="18" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="16" t="s">
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16" t="s">
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="18" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="19" t="s">
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="18" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="19"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="16" t="s">
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16" t="s">
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16" t="s">
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16" t="s">
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="17" t="s">
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+      <c r="AP2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AQ2" s="16"/>
-      <c r="AR2" s="16"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="15"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -11871,6 +11871,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="W1:AG1"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AH1:AR1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
     <mergeCell ref="L1:V1"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="P2:S2"/>
@@ -11879,14 +11887,6 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="W1:AG1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AH1:AR1"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11918,60 +11918,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16" t="s">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">

</xml_diff>